<commit_message>
fixed Asian Age Groups
</commit_message>
<xml_diff>
--- a/CDC Vital Population Statisitics/Datasets/sjc_site_populations_jail_pm_2010_2020.xlsx
+++ b/CDC Vital Population Statisitics/Datasets/sjc_site_populations_jail_pm_2010_2020.xlsx
@@ -161,13 +161,13 @@
     <t xml:space="preserve">pop_adult_female_API_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_young_any_ethnicity</t>
+    <t xml:space="preserve">pop_API_young_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_middle_any_ethnicity</t>
+    <t xml:space="preserve">pop_API_middle_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_older_any_ethnicity</t>
+    <t xml:space="preserve">pop_API_older_non_hispanic</t>
   </si>
   <si>
     <t xml:space="preserve">04019</t>

</xml_diff>